<commit_message>
Adding experiment to sequential folder
</commit_message>
<xml_diff>
--- a/TEST/SEQUENTIAL/7F_48_WELL_COMPLETE_FILLING_M9/tube_stock/0_tube_stock.xlsx
+++ b/TEST/SEQUENTIAL/7F_48_WELL_COMPLETE_FILLING_M9/tube_stock/0_tube_stock.xlsx
@@ -517,46 +517,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>64.40000000000001</v>
+        <v>667.4</v>
       </c>
       <c r="C2" t="n">
-        <v>1935.6</v>
+        <v>1332.6</v>
       </c>
       <c r="D2" t="n">
-        <v>1747.6</v>
+        <v>271</v>
       </c>
       <c r="E2" t="n">
-        <v>252.4</v>
+        <v>1729</v>
       </c>
       <c r="F2" t="n">
-        <v>1050.1</v>
+        <v>282.9</v>
       </c>
       <c r="G2" t="n">
-        <v>949.9</v>
+        <v>1717.1</v>
       </c>
       <c r="H2" t="n">
-        <v>1565.6</v>
+        <v>320.9</v>
       </c>
       <c r="I2" t="n">
-        <v>434.4</v>
+        <v>1679.1</v>
       </c>
       <c r="J2" t="n">
-        <v>1219.1</v>
+        <v>1931.5</v>
       </c>
       <c r="K2" t="n">
-        <v>780.9</v>
+        <v>68.5</v>
       </c>
       <c r="L2" t="n">
-        <v>1461</v>
+        <v>1718.8</v>
       </c>
       <c r="M2" t="n">
-        <v>539</v>
+        <v>281.2</v>
       </c>
       <c r="N2" t="n">
-        <v>762.1</v>
+        <v>1140</v>
       </c>
       <c r="O2" t="n">
-        <v>1237.9</v>
+        <v>860</v>
       </c>
     </row>
     <row r="3">
@@ -566,46 +566,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>856.9</v>
+        <v>1288.8</v>
       </c>
       <c r="C3" t="n">
-        <v>1143.1</v>
+        <v>711.2</v>
       </c>
       <c r="D3" t="n">
-        <v>1130.9</v>
+        <v>1329.5</v>
       </c>
       <c r="E3" t="n">
-        <v>869.1</v>
+        <v>670.5</v>
       </c>
       <c r="F3" t="n">
-        <v>760.9</v>
+        <v>1859.9</v>
       </c>
       <c r="G3" t="n">
-        <v>1239.1</v>
+        <v>140.1</v>
       </c>
       <c r="H3" t="n">
-        <v>99.8</v>
+        <v>1175.4</v>
       </c>
       <c r="I3" t="n">
-        <v>1900.2</v>
+        <v>824.6</v>
       </c>
       <c r="J3" t="n">
-        <v>1540.7</v>
+        <v>438.4</v>
       </c>
       <c r="K3" t="n">
-        <v>459.3</v>
+        <v>1561.6</v>
       </c>
       <c r="L3" t="n">
-        <v>1070</v>
+        <v>285.7</v>
       </c>
       <c r="M3" t="n">
-        <v>930</v>
+        <v>1714.3</v>
       </c>
       <c r="N3" t="n">
-        <v>235</v>
+        <v>479.3</v>
       </c>
       <c r="O3" t="n">
-        <v>1765</v>
+        <v>1520.7</v>
       </c>
     </row>
     <row r="4">
@@ -615,46 +615,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1693.6</v>
+        <v>1950.5</v>
       </c>
       <c r="C4" t="n">
-        <v>306.4</v>
+        <v>49.5</v>
       </c>
       <c r="D4" t="n">
-        <v>498.8</v>
+        <v>681.3</v>
       </c>
       <c r="E4" t="n">
-        <v>1501.2</v>
+        <v>1318.7</v>
       </c>
       <c r="F4" t="n">
-        <v>1747.7</v>
+        <v>596.1</v>
       </c>
       <c r="G4" t="n">
-        <v>252.3</v>
+        <v>1403.9</v>
       </c>
       <c r="H4" t="n">
-        <v>174.2</v>
+        <v>929.8</v>
       </c>
       <c r="I4" t="n">
-        <v>1825.8</v>
+        <v>1070.2</v>
       </c>
       <c r="J4" t="n">
-        <v>1075.7</v>
+        <v>649.8</v>
       </c>
       <c r="K4" t="n">
-        <v>924.3</v>
+        <v>1350.2</v>
       </c>
       <c r="L4" t="n">
-        <v>469.5</v>
+        <v>527.9</v>
       </c>
       <c r="M4" t="n">
-        <v>1530.5</v>
+        <v>1472.1</v>
       </c>
       <c r="N4" t="n">
-        <v>1324.2</v>
+        <v>1603.4</v>
       </c>
       <c r="O4" t="n">
-        <v>675.8</v>
+        <v>396.6</v>
       </c>
     </row>
     <row r="5">
@@ -664,46 +664,46 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1750.2</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>249.8</v>
+        <v>1935.6</v>
       </c>
       <c r="D5" t="n">
-        <v>1107.2</v>
+        <v>1747.6</v>
       </c>
       <c r="E5" t="n">
-        <v>892.8</v>
+        <v>252.4</v>
       </c>
       <c r="F5" t="n">
-        <v>1210.1</v>
+        <v>1050.1</v>
       </c>
       <c r="G5" t="n">
-        <v>789.9</v>
+        <v>949.9</v>
       </c>
       <c r="H5" t="n">
-        <v>403.3</v>
+        <v>1565.6</v>
       </c>
       <c r="I5" t="n">
-        <v>1596.7</v>
+        <v>434.4</v>
       </c>
       <c r="J5" t="n">
-        <v>1466.1</v>
+        <v>1219.1</v>
       </c>
       <c r="K5" t="n">
-        <v>533.9</v>
+        <v>780.9</v>
       </c>
       <c r="L5" t="n">
-        <v>819.8</v>
+        <v>1461</v>
       </c>
       <c r="M5" t="n">
-        <v>1180.2</v>
+        <v>539</v>
       </c>
       <c r="N5" t="n">
-        <v>301</v>
+        <v>762.1</v>
       </c>
       <c r="O5" t="n">
-        <v>1699</v>
+        <v>1237.9</v>
       </c>
     </row>
     <row r="6">
@@ -713,46 +713,46 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1380.6</v>
+        <v>382.7</v>
       </c>
       <c r="C6" t="n">
-        <v>619.4</v>
+        <v>1617.3</v>
       </c>
       <c r="D6" t="n">
-        <v>1919.2</v>
+        <v>858.3</v>
       </c>
       <c r="E6" t="n">
-        <v>80.8</v>
+        <v>1141.7</v>
       </c>
       <c r="F6" t="n">
-        <v>1481.5</v>
+        <v>1525.3</v>
       </c>
       <c r="G6" t="n">
-        <v>518.5</v>
+        <v>474.7</v>
       </c>
       <c r="H6" t="n">
-        <v>56.8</v>
+        <v>1857</v>
       </c>
       <c r="I6" t="n">
-        <v>1943.2</v>
+        <v>143</v>
       </c>
       <c r="J6" t="n">
-        <v>691.3</v>
+        <v>1359.5</v>
       </c>
       <c r="K6" t="n">
-        <v>1308.7</v>
+        <v>640.5</v>
       </c>
       <c r="L6" t="n">
-        <v>1230.8</v>
+        <v>1874.7</v>
       </c>
       <c r="M6" t="n">
-        <v>769.2</v>
+        <v>125.3</v>
       </c>
       <c r="N6" t="n">
-        <v>1230.6</v>
+        <v>1863</v>
       </c>
       <c r="O6" t="n">
-        <v>769.4</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7">
@@ -762,46 +762,46 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1665.3</v>
+        <v>1511</v>
       </c>
       <c r="C7" t="n">
-        <v>334.7</v>
+        <v>489</v>
       </c>
       <c r="D7" t="n">
-        <v>1459.8</v>
+        <v>1792</v>
       </c>
       <c r="E7" t="n">
-        <v>540.2</v>
+        <v>208</v>
       </c>
       <c r="F7" t="n">
-        <v>708.3</v>
+        <v>71.2</v>
       </c>
       <c r="G7" t="n">
-        <v>1291.7</v>
+        <v>1928.8</v>
       </c>
       <c r="H7" t="n">
-        <v>1530.4</v>
+        <v>647.2</v>
       </c>
       <c r="I7" t="n">
-        <v>469.6</v>
+        <v>1352.8</v>
       </c>
       <c r="J7" t="n">
-        <v>9.9</v>
+        <v>759</v>
       </c>
       <c r="K7" t="n">
-        <v>1990.1</v>
+        <v>1241</v>
       </c>
       <c r="L7" t="n">
-        <v>1363.3</v>
+        <v>182.8</v>
       </c>
       <c r="M7" t="n">
-        <v>636.7</v>
+        <v>1817.2</v>
       </c>
       <c r="N7" t="n">
-        <v>1766.4</v>
+        <v>521.6</v>
       </c>
       <c r="O7" t="n">
-        <v>233.6</v>
+        <v>1478.4</v>
       </c>
     </row>
     <row r="8">
@@ -811,46 +811,46 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1597.9</v>
+        <v>1220.5</v>
       </c>
       <c r="C8" t="n">
-        <v>402.1</v>
+        <v>779.5</v>
       </c>
       <c r="D8" t="n">
-        <v>752.9</v>
+        <v>189.5</v>
       </c>
       <c r="E8" t="n">
-        <v>1247.1</v>
+        <v>1810.5</v>
       </c>
       <c r="F8" t="n">
-        <v>1094</v>
+        <v>1338.1</v>
       </c>
       <c r="G8" t="n">
-        <v>906</v>
+        <v>661.9</v>
       </c>
       <c r="H8" t="n">
-        <v>1058.4</v>
+        <v>1403.4</v>
       </c>
       <c r="I8" t="n">
-        <v>941.6</v>
+        <v>596.6</v>
       </c>
       <c r="J8" t="n">
-        <v>1826.6</v>
+        <v>78.8</v>
       </c>
       <c r="K8" t="n">
-        <v>173.4</v>
+        <v>1921.2</v>
       </c>
       <c r="L8" t="n">
-        <v>1039.1</v>
+        <v>878.1</v>
       </c>
       <c r="M8" t="n">
-        <v>960.9</v>
+        <v>1121.9</v>
       </c>
       <c r="N8" t="n">
-        <v>75.40000000000001</v>
+        <v>1395.6</v>
       </c>
       <c r="O8" t="n">
-        <v>1924.6</v>
+        <v>604.4</v>
       </c>
     </row>
     <row r="9">

</xml_diff>